<commit_message>
Added Sense Conversion to auto_merger
</commit_message>
<xml_diff>
--- a/Retinal_Candidate_Set/D_rerio_RARE_List.xlsx
+++ b/Retinal_Candidate_Set/D_rerio_RARE_List.xlsx
@@ -695,7 +695,58 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -975,8 +1026,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1028,7 +1079,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1045,7 +1096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1062,7 +1113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1130,7 +1181,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -1147,7 +1198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1164,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1238,7 +1289,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1261,7 +1312,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1284,7 +1335,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1307,7 +1358,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1500,7 +1551,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1523,7 +1574,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -1546,7 +1597,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1569,7 +1620,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1748,7 +1799,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1819,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -1788,7 +1839,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -1808,7 +1859,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1828,7 +1879,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -1848,7 +1899,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -1868,7 +1919,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1888,7 +1939,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1905,7 +1956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1922,7 +1973,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -1939,7 +1990,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1956,7 +2007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1973,7 +2024,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1990,7 +2041,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2007,7 +2058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2024,7 +2075,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -2041,7 +2092,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -2058,7 +2109,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -2075,7 +2126,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -2092,7 +2143,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>53</v>
       </c>
@@ -2109,7 +2160,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -2126,7 +2177,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -2143,7 +2194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -2177,7 +2228,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -2228,7 +2279,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -2248,7 +2299,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>86</v>
       </c>
@@ -2268,7 +2319,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -2302,7 +2353,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>86</v>
       </c>
@@ -2353,7 +2404,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>95</v>
       </c>
@@ -2404,7 +2455,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>95</v>
       </c>
@@ -2441,7 +2492,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -2461,7 +2512,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>100</v>
       </c>
@@ -2498,7 +2549,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>100</v>
       </c>
@@ -2532,7 +2583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>108</v>
       </c>
@@ -2589,7 +2640,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>108</v>
       </c>
@@ -2708,7 +2759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -2742,7 +2793,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>108</v>
       </c>
@@ -2776,7 +2827,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -2878,7 +2929,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -2997,7 +3048,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>108</v>
       </c>
@@ -3099,7 +3150,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>108</v>
       </c>
@@ -3201,7 +3252,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>108</v>
       </c>
@@ -3303,7 +3354,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>108</v>
       </c>
@@ -3320,7 +3371,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>127</v>
       </c>
@@ -3340,7 +3391,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>127</v>
       </c>
@@ -3380,7 +3431,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>131</v>
       </c>
@@ -3400,7 +3451,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -3420,7 +3471,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -3588,7 +3639,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>134</v>
       </c>
@@ -3605,7 +3656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -3639,7 +3690,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -3656,7 +3707,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -3741,7 +3792,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>145</v>
       </c>
@@ -3775,7 +3826,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>145</v>
       </c>
@@ -3809,7 +3860,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>145</v>
       </c>
@@ -3826,7 +3877,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>145</v>
       </c>
@@ -3843,7 +3894,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>145</v>
       </c>
@@ -3877,7 +3928,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>145</v>
       </c>
@@ -3894,7 +3945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>145</v>
       </c>
@@ -3911,7 +3962,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>145</v>
       </c>
@@ -3945,7 +3996,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>145</v>
       </c>
@@ -3962,7 +4013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>145</v>
       </c>
@@ -3979,7 +4030,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>145</v>
       </c>
@@ -4013,7 +4064,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>145</v>
       </c>
@@ -4030,7 +4081,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>145</v>
       </c>
@@ -4047,7 +4098,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>145</v>
       </c>
@@ -4081,7 +4132,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>145</v>
       </c>
@@ -4098,7 +4149,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>145</v>
       </c>
@@ -4149,7 +4200,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>145</v>
       </c>
@@ -4183,7 +4234,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>162</v>
       </c>
@@ -4263,7 +4314,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>168</v>
       </c>
@@ -4303,7 +4354,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>170</v>
       </c>
@@ -4325,10 +4376,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E187">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter val="*NM*"/>
-      </customFilters>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Forward Coding"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <hyperlinks>

</xml_diff>